<commit_message>
Actualización 26 Abril 2021
</commit_message>
<xml_diff>
--- a/Calificaciones.xlsx
+++ b/Calificaciones.xlsx
@@ -399,7 +399,7 @@
     <t>URBANO GARCIA EVELYN</t>
   </si>
   <si>
-    <t>VAZQUEZ HERNANDEZ VICTOR MANUEL</t>
+    <t>VASQUEZ HERNANDEZ VICTOR MANUEL</t>
   </si>
   <si>
     <t>VERA PONCE MARITZA</t>
@@ -651,6 +651,9 @@
     <t>CABRERA RODRIGUEZ DANIEL</t>
   </si>
   <si>
+    <t>CAMARILLO SORIA ARIZBET</t>
+  </si>
+  <si>
     <t>CARAZA CRUZ JARED URIEL</t>
   </si>
   <si>
@@ -724,9 +727,6 @@
   </si>
   <si>
     <t>ROJAS ROJAS DULCE MARIA</t>
-  </si>
-  <si>
-    <t>SORIA CAMARILLO ARIZBET</t>
   </si>
   <si>
     <t>TORRES CARRASCO ZULEICA RENATA</t>
@@ -63410,22 +63410,22 @@
         <v>201</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D9">
-        <v>10</v>
+        <v>-1</v>
       </c>
       <c r="E9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="G9">
-        <v>8</v>
+        <v>-1</v>
       </c>
       <c r="H9">
         <v>-1</v>
@@ -63469,7 +63469,7 @@
         <v>202</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10">
         <v>10</v>
@@ -63481,10 +63481,10 @@
         <v>9</v>
       </c>
       <c r="F10">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G10">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H10">
         <v>-1</v>
@@ -63528,22 +63528,22 @@
         <v>203</v>
       </c>
       <c r="B11">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D11">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="E11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F11">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="G11">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="H11">
         <v>-1</v>
@@ -63587,19 +63587,19 @@
         <v>204</v>
       </c>
       <c r="B12">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="C12">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D12">
-        <v>9</v>
+        <v>-1</v>
       </c>
       <c r="E12">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F12">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="G12">
         <v>-1</v>
@@ -63646,19 +63646,19 @@
         <v>205</v>
       </c>
       <c r="B13">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D13">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="E13">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="F13">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="G13">
         <v>-1</v>
@@ -63705,22 +63705,22 @@
         <v>206</v>
       </c>
       <c r="B14">
-        <v>8</v>
+        <v>-1</v>
       </c>
       <c r="C14">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>-1</v>
       </c>
       <c r="E14">
-        <v>10</v>
+        <v>-1</v>
       </c>
       <c r="F14">
-        <v>8</v>
+        <v>-1</v>
       </c>
       <c r="G14">
-        <v>7</v>
+        <v>-1</v>
       </c>
       <c r="H14">
         <v>-1</v>
@@ -63764,10 +63764,10 @@
         <v>207</v>
       </c>
       <c r="B15">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C15">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D15">
         <v>10</v>
@@ -63776,10 +63776,10 @@
         <v>10</v>
       </c>
       <c r="F15">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G15">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H15">
         <v>-1</v>
@@ -63829,16 +63829,16 @@
         <v>9</v>
       </c>
       <c r="D16">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E16">
         <v>10</v>
       </c>
       <c r="F16">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G16">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H16">
         <v>-1</v>
@@ -63882,19 +63882,19 @@
         <v>209</v>
       </c>
       <c r="B17">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C17">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D17">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E17">
         <v>10</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G17">
         <v>9</v>
@@ -63941,22 +63941,22 @@
         <v>210</v>
       </c>
       <c r="B18">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D18">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E18">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F18">
         <v>6</v>
       </c>
       <c r="G18">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H18">
         <v>-1</v>
@@ -64000,22 +64000,22 @@
         <v>211</v>
       </c>
       <c r="B19">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C19">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D19">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="E19">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F19">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G19">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H19">
         <v>-1</v>
@@ -64059,10 +64059,10 @@
         <v>212</v>
       </c>
       <c r="B20">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="C20">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D20">
         <v>-1</v>
@@ -64071,10 +64071,10 @@
         <v>6</v>
       </c>
       <c r="F20">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G20">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="H20">
         <v>-1</v>
@@ -64127,10 +64127,10 @@
         <v>-1</v>
       </c>
       <c r="E21">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="F21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G21">
         <v>-1</v>
@@ -64177,22 +64177,22 @@
         <v>214</v>
       </c>
       <c r="B22">
-        <v>7</v>
+        <v>-1</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D22">
-        <v>8</v>
+        <v>-1</v>
       </c>
       <c r="E22">
-        <v>10</v>
+        <v>-1</v>
       </c>
       <c r="F22">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G22">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="H22">
         <v>-1</v>
@@ -64236,22 +64236,22 @@
         <v>215</v>
       </c>
       <c r="B23">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D23">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="E23">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F23">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="G23">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="H23">
         <v>-1</v>
@@ -64295,19 +64295,19 @@
         <v>216</v>
       </c>
       <c r="B24">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="C24">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D24">
         <v>-1</v>
       </c>
       <c r="E24">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F24">
-        <v>7</v>
+        <v>-1</v>
       </c>
       <c r="G24">
         <v>-1</v>
@@ -64357,16 +64357,16 @@
         <v>6</v>
       </c>
       <c r="C25">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D25">
         <v>-1</v>
       </c>
       <c r="E25">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="F25">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G25">
         <v>-1</v>
@@ -64413,19 +64413,19 @@
         <v>218</v>
       </c>
       <c r="B26">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="C26">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D26">
         <v>-1</v>
       </c>
       <c r="E26">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="F26">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="G26">
         <v>-1</v>
@@ -64472,22 +64472,22 @@
         <v>219</v>
       </c>
       <c r="B27">
-        <v>10</v>
+        <v>-1</v>
       </c>
       <c r="C27">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D27">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="E27">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F27">
-        <v>7</v>
+        <v>-1</v>
       </c>
       <c r="G27">
-        <v>10</v>
+        <v>-1</v>
       </c>
       <c r="H27">
         <v>-1</v>
@@ -64531,22 +64531,22 @@
         <v>220</v>
       </c>
       <c r="B28">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C28">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D28">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="E28">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F28">
         <v>7</v>
       </c>
       <c r="G28">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H28">
         <v>-1</v>
@@ -64590,22 +64590,22 @@
         <v>221</v>
       </c>
       <c r="B29">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="C29">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D29">
-        <v>7</v>
+        <v>-1</v>
       </c>
       <c r="E29">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F29">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="G29">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="H29">
         <v>-1</v>
@@ -64649,22 +64649,22 @@
         <v>222</v>
       </c>
       <c r="B30">
-        <v>9</v>
+        <v>-1</v>
       </c>
       <c r="C30">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D30">
         <v>7</v>
       </c>
       <c r="E30">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F30">
-        <v>7</v>
+        <v>-1</v>
       </c>
       <c r="G30">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="H30">
         <v>-1</v>
@@ -64708,22 +64708,22 @@
         <v>223</v>
       </c>
       <c r="B31">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C31">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D31">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E31">
         <v>10</v>
       </c>
       <c r="F31">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G31">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H31">
         <v>-1</v>
@@ -64776,13 +64776,13 @@
         <v>6</v>
       </c>
       <c r="E32">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F32">
         <v>6</v>
       </c>
       <c r="G32">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="H32">
         <v>-1</v>
@@ -64829,19 +64829,19 @@
         <v>6</v>
       </c>
       <c r="C33">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D33">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E33">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F33">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G33">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="H33">
         <v>-1</v>
@@ -64888,19 +64888,19 @@
         <v>6</v>
       </c>
       <c r="C34">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D34">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="E34">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F34">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="G34">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="H34">
         <v>-1</v>

</xml_diff>

<commit_message>
Actualización 11 de Mayo - Tarde
</commit_message>
<xml_diff>
--- a/Calificaciones.xlsx
+++ b/Calificaciones.xlsx
@@ -7827,7 +7827,7 @@
         <v>9</v>
       </c>
       <c r="L4">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="M4">
         <v>10</v>
@@ -7895,7 +7895,7 @@
         <v>7</v>
       </c>
       <c r="L5">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="M5">
         <v>7</v>
@@ -7963,7 +7963,7 @@
         <v>8</v>
       </c>
       <c r="L6">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="M6">
         <v>9</v>
@@ -8031,7 +8031,7 @@
         <v>9</v>
       </c>
       <c r="L7">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="M7">
         <v>10</v>
@@ -8099,7 +8099,7 @@
         <v>8</v>
       </c>
       <c r="L8">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="M8">
         <v>9</v>
@@ -8167,7 +8167,7 @@
         <v>-1</v>
       </c>
       <c r="L9">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="M9">
         <v>-1</v>
@@ -8235,7 +8235,7 @@
         <v>-1</v>
       </c>
       <c r="L10">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="M10">
         <v>-1</v>
@@ -8303,7 +8303,7 @@
         <v>7</v>
       </c>
       <c r="L11">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="M11">
         <v>6</v>
@@ -8371,7 +8371,7 @@
         <v>-1</v>
       </c>
       <c r="L12">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="M12">
         <v>-1</v>
@@ -8439,7 +8439,7 @@
         <v>-1</v>
       </c>
       <c r="L13">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="M13">
         <v>-1</v>
@@ -8507,7 +8507,7 @@
         <v>-1</v>
       </c>
       <c r="L14">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="M14">
         <v>-1</v>
@@ -8575,7 +8575,7 @@
         <v>9</v>
       </c>
       <c r="L15">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="M15">
         <v>9</v>
@@ -8643,7 +8643,7 @@
         <v>-1</v>
       </c>
       <c r="L16">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="M16">
         <v>-1</v>
@@ -8711,7 +8711,7 @@
         <v>-1</v>
       </c>
       <c r="L17">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="M17">
         <v>-1</v>
@@ -8779,7 +8779,7 @@
         <v>7</v>
       </c>
       <c r="L18">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="M18">
         <v>10</v>
@@ -8847,7 +8847,7 @@
         <v>-1</v>
       </c>
       <c r="L19">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="M19">
         <v>-1</v>
@@ -8915,7 +8915,7 @@
         <v>-1</v>
       </c>
       <c r="L20">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="M20">
         <v>8</v>
@@ -8983,7 +8983,7 @@
         <v>7</v>
       </c>
       <c r="L21">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="M21">
         <v>9</v>
@@ -9051,7 +9051,7 @@
         <v>6</v>
       </c>
       <c r="L22">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="M22">
         <v>8</v>
@@ -9119,7 +9119,7 @@
         <v>10</v>
       </c>
       <c r="L23">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="M23">
         <v>10</v>
@@ -9187,7 +9187,7 @@
         <v>9</v>
       </c>
       <c r="L24">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="M24">
         <v>8</v>
@@ -9255,7 +9255,7 @@
         <v>-1</v>
       </c>
       <c r="L25">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="M25">
         <v>-1</v>
@@ -9323,7 +9323,7 @@
         <v>-1</v>
       </c>
       <c r="L26">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="M26">
         <v>-1</v>
@@ -9391,7 +9391,7 @@
         <v>7</v>
       </c>
       <c r="L27">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="M27">
         <v>7</v>
@@ -9459,7 +9459,7 @@
         <v>6</v>
       </c>
       <c r="L28">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="M28">
         <v>-1</v>
@@ -9527,7 +9527,7 @@
         <v>-1</v>
       </c>
       <c r="L29">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="M29">
         <v>-1</v>
@@ -9595,7 +9595,7 @@
         <v>-1</v>
       </c>
       <c r="L30">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="M30">
         <v>6</v>
@@ -9663,7 +9663,7 @@
         <v>7</v>
       </c>
       <c r="L31">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="M31">
         <v>6</v>
@@ -9731,7 +9731,7 @@
         <v>9</v>
       </c>
       <c r="L32">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="M32">
         <v>7</v>
@@ -9799,7 +9799,7 @@
         <v>-1</v>
       </c>
       <c r="L33">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="M33">
         <v>-1</v>
@@ -9867,7 +9867,7 @@
         <v>9</v>
       </c>
       <c r="L34">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="M34">
         <v>-1</v>
@@ -9935,7 +9935,7 @@
         <v>6</v>
       </c>
       <c r="L35">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="M35">
         <v>8</v>
@@ -10003,7 +10003,7 @@
         <v>7</v>
       </c>
       <c r="L36">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="M36">
         <v>8</v>
@@ -10071,7 +10071,7 @@
         <v>-1</v>
       </c>
       <c r="L37">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="M37">
         <v>-1</v>
@@ -10139,7 +10139,7 @@
         <v>9</v>
       </c>
       <c r="L38">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="M38">
         <v>10</v>
@@ -10207,7 +10207,7 @@
         <v>6</v>
       </c>
       <c r="L39">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="M39">
         <v>9</v>
@@ -10275,7 +10275,7 @@
         <v>-1</v>
       </c>
       <c r="L40">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="M40">
         <v>-1</v>
@@ -10467,7 +10467,7 @@
         <v>9</v>
       </c>
       <c r="L4">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="M4">
         <v>10</v>
@@ -10535,7 +10535,7 @@
         <v>9</v>
       </c>
       <c r="L5">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="M5">
         <v>10</v>
@@ -10603,7 +10603,7 @@
         <v>9</v>
       </c>
       <c r="L6">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="M6">
         <v>8</v>
@@ -10671,7 +10671,7 @@
         <v>-1</v>
       </c>
       <c r="L7">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -10739,7 +10739,7 @@
         <v>9</v>
       </c>
       <c r="L8">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="M8">
         <v>10</v>
@@ -10807,7 +10807,7 @@
         <v>9</v>
       </c>
       <c r="L9">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="M9">
         <v>10</v>
@@ -10875,7 +10875,7 @@
         <v>9</v>
       </c>
       <c r="L10">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="M10">
         <v>9</v>
@@ -10943,7 +10943,7 @@
         <v>8</v>
       </c>
       <c r="L11">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="M11">
         <v>10</v>
@@ -11011,7 +11011,7 @@
         <v>-1</v>
       </c>
       <c r="L12">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="M12">
         <v>5</v>
@@ -11079,7 +11079,7 @@
         <v>-1</v>
       </c>
       <c r="L13">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -11147,7 +11147,7 @@
         <v>7</v>
       </c>
       <c r="L14">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="M14">
         <v>10</v>
@@ -11215,7 +11215,7 @@
         <v>-1</v>
       </c>
       <c r="L15">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="M15">
         <v>5</v>
@@ -11283,7 +11283,7 @@
         <v>9</v>
       </c>
       <c r="L16">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="M16">
         <v>5</v>
@@ -11351,7 +11351,7 @@
         <v>8</v>
       </c>
       <c r="L17">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="M17">
         <v>9</v>
@@ -11419,7 +11419,7 @@
         <v>9</v>
       </c>
       <c r="L18">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="M18">
         <v>9</v>
@@ -11487,7 +11487,7 @@
         <v>-1</v>
       </c>
       <c r="L19">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="M19">
         <v>9</v>
@@ -11555,7 +11555,7 @@
         <v>8</v>
       </c>
       <c r="L20">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="M20">
         <v>9</v>
@@ -11623,7 +11623,7 @@
         <v>6</v>
       </c>
       <c r="L21">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="M21">
         <v>9</v>
@@ -11691,7 +11691,7 @@
         <v>-1</v>
       </c>
       <c r="L22">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="M22">
         <v>5</v>
@@ -11759,7 +11759,7 @@
         <v>6</v>
       </c>
       <c r="L23">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="M23">
         <v>8</v>
@@ -11827,7 +11827,7 @@
         <v>-1</v>
       </c>
       <c r="L24">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="M24">
         <v>8</v>
@@ -11895,7 +11895,7 @@
         <v>-1</v>
       </c>
       <c r="L25">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="M25">
         <v>5</v>
@@ -11963,7 +11963,7 @@
         <v>9</v>
       </c>
       <c r="L26">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="M26">
         <v>7</v>
@@ -12031,7 +12031,7 @@
         <v>-1</v>
       </c>
       <c r="L27">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="M27">
         <v>5</v>
@@ -12099,7 +12099,7 @@
         <v>10</v>
       </c>
       <c r="L28">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="M28">
         <v>10</v>
@@ -12167,7 +12167,7 @@
         <v>9</v>
       </c>
       <c r="L29">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="M29">
         <v>8</v>
@@ -12235,7 +12235,7 @@
         <v>9</v>
       </c>
       <c r="L30">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="M30">
         <v>10</v>
@@ -12303,7 +12303,7 @@
         <v>6</v>
       </c>
       <c r="L31">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="M31">
         <v>10</v>
@@ -12371,7 +12371,7 @@
         <v>7</v>
       </c>
       <c r="L32">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="M32">
         <v>5</v>
@@ -12439,7 +12439,7 @@
         <v>9</v>
       </c>
       <c r="L33">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="M33">
         <v>10</v>
@@ -12507,7 +12507,7 @@
         <v>-1</v>
       </c>
       <c r="L34">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="M34">
         <v>5</v>
@@ -12575,7 +12575,7 @@
         <v>9</v>
       </c>
       <c r="L35">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="M35">
         <v>9</v>
@@ -12643,7 +12643,7 @@
         <v>9</v>
       </c>
       <c r="L36">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="M36">
         <v>10</v>
@@ -12711,7 +12711,7 @@
         <v>9</v>
       </c>
       <c r="L37">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="M37">
         <v>10</v>
@@ -12779,7 +12779,7 @@
         <v>-1</v>
       </c>
       <c r="L38">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="M38">
         <v>10</v>
@@ -12847,7 +12847,7 @@
         <v>8</v>
       </c>
       <c r="L39">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="M39">
         <v>9</v>
@@ -19201,7 +19201,7 @@
         <v>-1</v>
       </c>
       <c r="K9">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="L9">
         <v>-1</v>
@@ -19378,7 +19378,7 @@
         <v>7</v>
       </c>
       <c r="K12">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="L12">
         <v>-1</v>
@@ -19850,7 +19850,7 @@
         <v>-1</v>
       </c>
       <c r="K20">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="L20">
         <v>6</v>
@@ -48855,7 +48855,7 @@
         <v>8</v>
       </c>
       <c r="L4">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="M4">
         <v>9</v>
@@ -48914,7 +48914,7 @@
         <v>7</v>
       </c>
       <c r="L5">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="M5">
         <v>7</v>
@@ -48973,7 +48973,7 @@
         <v>9</v>
       </c>
       <c r="L6">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="M6">
         <v>6</v>
@@ -49150,7 +49150,7 @@
         <v>7</v>
       </c>
       <c r="L9">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="M9">
         <v>8</v>
@@ -49268,7 +49268,7 @@
         <v>10</v>
       </c>
       <c r="L11">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="M11">
         <v>8</v>
@@ -49386,7 +49386,7 @@
         <v>8</v>
       </c>
       <c r="L13">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="M13">
         <v>5</v>
@@ -49445,7 +49445,7 @@
         <v>10</v>
       </c>
       <c r="L14">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="M14">
         <v>8</v>
@@ -49504,7 +49504,7 @@
         <v>10</v>
       </c>
       <c r="L15">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="M15">
         <v>8</v>
@@ -49681,7 +49681,7 @@
         <v>9</v>
       </c>
       <c r="L18">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="M18">
         <v>7</v>
@@ -49740,7 +49740,7 @@
         <v>7</v>
       </c>
       <c r="L19">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="M19">
         <v>6</v>
@@ -49917,7 +49917,7 @@
         <v>7</v>
       </c>
       <c r="L22">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="M22">
         <v>6</v>
@@ -49976,7 +49976,7 @@
         <v>8</v>
       </c>
       <c r="L23">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="M23">
         <v>8</v>
@@ -50035,7 +50035,7 @@
         <v>6</v>
       </c>
       <c r="L24">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="M24">
         <v>6</v>
@@ -50271,7 +50271,7 @@
         <v>7</v>
       </c>
       <c r="L28">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="M28">
         <v>7</v>
@@ -70818,7 +70818,7 @@
         <v>6</v>
       </c>
       <c r="O4">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="P4">
         <v>-1</v>
@@ -70886,7 +70886,7 @@
         <v>7</v>
       </c>
       <c r="O5">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="P5">
         <v>-1</v>
@@ -70954,7 +70954,7 @@
         <v>-1</v>
       </c>
       <c r="O6">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="P6">
         <v>-1</v>
@@ -71022,7 +71022,7 @@
         <v>9</v>
       </c>
       <c r="O7">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="P7">
         <v>-1</v>
@@ -71090,7 +71090,7 @@
         <v>6</v>
       </c>
       <c r="O8">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="P8">
         <v>-1</v>
@@ -71158,7 +71158,7 @@
         <v>-1</v>
       </c>
       <c r="O9">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="P9">
         <v>-1</v>
@@ -71226,7 +71226,7 @@
         <v>-1</v>
       </c>
       <c r="O10">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="P10">
         <v>-1</v>
@@ -71294,7 +71294,7 @@
         <v>6</v>
       </c>
       <c r="O11">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="P11">
         <v>-1</v>
@@ -71362,7 +71362,7 @@
         <v>7</v>
       </c>
       <c r="O12">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="P12">
         <v>-1</v>
@@ -71430,7 +71430,7 @@
         <v>-1</v>
       </c>
       <c r="O13">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="P13">
         <v>-1</v>
@@ -71498,7 +71498,7 @@
         <v>-1</v>
       </c>
       <c r="O14">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="P14">
         <v>-1</v>
@@ -71566,7 +71566,7 @@
         <v>-1</v>
       </c>
       <c r="O15">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="P15">
         <v>-1</v>
@@ -71634,7 +71634,7 @@
         <v>-1</v>
       </c>
       <c r="O16">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="P16">
         <v>-1</v>
@@ -71702,7 +71702,7 @@
         <v>-1</v>
       </c>
       <c r="O17">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="P17">
         <v>-1</v>
@@ -71770,7 +71770,7 @@
         <v>-1</v>
       </c>
       <c r="O18">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="P18">
         <v>-1</v>
@@ -71838,7 +71838,7 @@
         <v>-1</v>
       </c>
       <c r="O19">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="P19">
         <v>-1</v>
@@ -71906,7 +71906,7 @@
         <v>-1</v>
       </c>
       <c r="O20">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="P20">
         <v>-1</v>
@@ -71974,7 +71974,7 @@
         <v>-1</v>
       </c>
       <c r="O21">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="P21">
         <v>-1</v>
@@ -72042,7 +72042,7 @@
         <v>8</v>
       </c>
       <c r="O22">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="P22">
         <v>-1</v>
@@ -72110,7 +72110,7 @@
         <v>6</v>
       </c>
       <c r="O23">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="P23">
         <v>-1</v>
@@ -72178,7 +72178,7 @@
         <v>8</v>
       </c>
       <c r="O24">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="P24">
         <v>-1</v>
@@ -72246,7 +72246,7 @@
         <v>10</v>
       </c>
       <c r="O25">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="P25">
         <v>-1</v>
@@ -72314,7 +72314,7 @@
         <v>-1</v>
       </c>
       <c r="O26">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="P26">
         <v>-1</v>
@@ -72382,7 +72382,7 @@
         <v>6</v>
       </c>
       <c r="O27">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="P27">
         <v>-1</v>
@@ -72450,7 +72450,7 @@
         <v>-1</v>
       </c>
       <c r="O28">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="P28">
         <v>-1</v>
@@ -72518,7 +72518,7 @@
         <v>-1</v>
       </c>
       <c r="O29">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="P29">
         <v>-1</v>
@@ -72586,7 +72586,7 @@
         <v>6</v>
       </c>
       <c r="O30">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="P30">
         <v>-1</v>
@@ -72654,7 +72654,7 @@
         <v>-1</v>
       </c>
       <c r="O31">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="P31">
         <v>-1</v>

</xml_diff>

<commit_message>
11 May - Noche
</commit_message>
<xml_diff>
--- a/Calificaciones.xlsx
+++ b/Calificaciones.xlsx
@@ -2376,10 +2376,10 @@
     <t>RODRIGUEZ BARRAGAN LUCERO</t>
   </si>
   <si>
+    <t>ROSAS SALAZAR MARIA FERNANDA</t>
+  </si>
+  <si>
     <t>RUIZ LOPEZ XIMENA MICHELL</t>
-  </si>
-  <si>
-    <t>SALAZAR MARIA FERNANDA ROSAS</t>
   </si>
   <si>
     <t>SANCHEZ RAMON MEILYN ADABEL</t>
@@ -34991,40 +34991,40 @@
         <v>776</v>
       </c>
       <c r="B36">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C36">
         <v>10</v>
       </c>
       <c r="D36">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E36">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F36">
         <v>8</v>
       </c>
       <c r="G36">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H36">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I36">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J36">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K36">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L36">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M36">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N36">
         <v>-1</v>
@@ -35050,40 +35050,40 @@
         <v>777</v>
       </c>
       <c r="B37">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C37">
         <v>10</v>
       </c>
       <c r="D37">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E37">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F37">
         <v>8</v>
       </c>
       <c r="G37">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H37">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I37">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J37">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K37">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L37">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M37">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N37">
         <v>-1</v>

</xml_diff>

<commit_message>
Nuevo formato 15 jun 2021
</commit_message>
<xml_diff>
--- a/Calificaciones.xlsx
+++ b/Calificaciones.xlsx
@@ -24809,7 +24809,7 @@
         <v>5</v>
       </c>
       <c r="N21">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="O21">
         <v>5</v>
@@ -35769,13 +35769,13 @@
         <v>5</v>
       </c>
       <c r="Q25">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="R25">
         <v>-1</v>
       </c>
       <c r="S25">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="T25">
         <v>6</v>
@@ -35787,7 +35787,7 @@
         <v>6</v>
       </c>
       <c r="W25">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="X25">
         <v>7</v>
@@ -36000,7 +36000,7 @@
         <v>6</v>
       </c>
       <c r="Q28">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="R28">
         <v>-1</v>
@@ -36018,7 +36018,7 @@
         <v>6</v>
       </c>
       <c r="W28">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="X28">
         <v>7</v>
@@ -36450,7 +36450,7 @@
         <v>7</v>
       </c>
       <c r="M34">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="N34">
         <v>5</v>
@@ -36462,13 +36462,13 @@
         <v>5</v>
       </c>
       <c r="Q34">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="R34">
         <v>-1</v>
       </c>
       <c r="S34">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="T34">
         <v>5</v>
@@ -36480,13 +36480,13 @@
         <v>5</v>
       </c>
       <c r="W34">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="X34">
         <v>9</v>
       </c>
       <c r="Y34">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:25">
@@ -40016,13 +40016,13 @@
         <v>10</v>
       </c>
       <c r="P4">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="Q4">
         <v>9</v>
       </c>
       <c r="R4">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="S4">
         <v>9</v>
@@ -40037,7 +40037,7 @@
         <v>10</v>
       </c>
       <c r="W4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="X4">
         <v>9</v>
@@ -40063,13 +40063,13 @@
         <v>725</v>
       </c>
       <c r="B5">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>6</v>
       </c>
       <c r="D5">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="E5">
         <v>6</v>
@@ -40084,13 +40084,13 @@
         <v>6</v>
       </c>
       <c r="I5">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="J5">
         <v>6</v>
       </c>
       <c r="K5">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="L5">
         <v>5</v>
@@ -40105,13 +40105,13 @@
         <v>5</v>
       </c>
       <c r="P5">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Q5">
         <v>6</v>
       </c>
       <c r="R5">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="S5">
         <v>7</v>
@@ -40126,13 +40126,13 @@
         <v>7</v>
       </c>
       <c r="W5">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="X5">
         <v>6</v>
       </c>
       <c r="Y5">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Z5">
         <v>6</v>
@@ -40194,13 +40194,13 @@
         <v>10</v>
       </c>
       <c r="P6">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="Q6">
         <v>10</v>
       </c>
       <c r="R6">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="S6">
         <v>10</v>
@@ -40283,13 +40283,13 @@
         <v>9</v>
       </c>
       <c r="P7">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="Q7">
         <v>6</v>
       </c>
       <c r="R7">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="S7">
         <v>8</v>
@@ -40304,7 +40304,7 @@
         <v>9</v>
       </c>
       <c r="W7">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="X7">
         <v>7</v>
@@ -40372,13 +40372,13 @@
         <v>5</v>
       </c>
       <c r="P8">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Q8">
         <v>6</v>
       </c>
       <c r="R8">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="S8">
         <v>-1</v>
@@ -40393,13 +40393,13 @@
         <v>7</v>
       </c>
       <c r="W8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="X8">
         <v>6</v>
       </c>
       <c r="Y8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Z8">
         <v>5</v>
@@ -40461,13 +40461,13 @@
         <v>5</v>
       </c>
       <c r="P9">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Q9">
         <v>6</v>
       </c>
       <c r="R9">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="S9">
         <v>5</v>
@@ -40482,13 +40482,13 @@
         <v>7</v>
       </c>
       <c r="W9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="X9">
         <v>6</v>
       </c>
       <c r="Y9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Z9">
         <v>6</v>
@@ -40550,13 +40550,13 @@
         <v>5</v>
       </c>
       <c r="P10">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="Q10">
         <v>8</v>
       </c>
       <c r="R10">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="S10">
         <v>8</v>
@@ -40577,7 +40577,7 @@
         <v>7</v>
       </c>
       <c r="Y10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Z10">
         <v>7</v>
@@ -40686,13 +40686,13 @@
         <v>732</v>
       </c>
       <c r="B12">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="C12">
         <v>6</v>
       </c>
       <c r="D12">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="E12">
         <v>5</v>
@@ -40707,13 +40707,13 @@
         <v>5</v>
       </c>
       <c r="I12">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="J12">
         <v>6</v>
       </c>
       <c r="K12">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="L12">
         <v>-1</v>
@@ -40728,13 +40728,13 @@
         <v>5</v>
       </c>
       <c r="P12">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Q12">
         <v>6</v>
       </c>
       <c r="R12">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="S12">
         <v>-1</v>
@@ -40749,13 +40749,13 @@
         <v>8</v>
       </c>
       <c r="W12">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="X12">
         <v>6</v>
       </c>
       <c r="Y12">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Z12">
         <v>5</v>
@@ -40817,13 +40817,13 @@
         <v>7</v>
       </c>
       <c r="P13">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="Q13">
         <v>8</v>
       </c>
       <c r="R13">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="S13">
         <v>5</v>
@@ -40844,7 +40844,7 @@
         <v>7</v>
       </c>
       <c r="Y13">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Z13">
         <v>7</v>
@@ -40906,13 +40906,13 @@
         <v>9</v>
       </c>
       <c r="P14">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="Q14">
         <v>9</v>
       </c>
       <c r="R14">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="S14">
         <v>10</v>
@@ -40995,13 +40995,13 @@
         <v>9</v>
       </c>
       <c r="P15">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="Q15">
         <v>8</v>
       </c>
       <c r="R15">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="S15">
         <v>7</v>
@@ -41084,13 +41084,13 @@
         <v>9</v>
       </c>
       <c r="P16">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="Q16">
         <v>8</v>
       </c>
       <c r="R16">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="S16">
         <v>8</v>
@@ -41173,13 +41173,13 @@
         <v>10</v>
       </c>
       <c r="P17">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="Q17">
         <v>7</v>
       </c>
       <c r="R17">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="S17">
         <v>10</v>
@@ -41220,13 +41220,13 @@
         <v>738</v>
       </c>
       <c r="B18">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="C18">
         <v>6</v>
       </c>
       <c r="D18">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="E18">
         <v>5</v>
@@ -41241,13 +41241,13 @@
         <v>6</v>
       </c>
       <c r="I18">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="J18">
         <v>6</v>
       </c>
       <c r="K18">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="L18">
         <v>6</v>
@@ -41262,13 +41262,13 @@
         <v>9</v>
       </c>
       <c r="P18">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Q18">
         <v>8</v>
       </c>
       <c r="R18">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="S18">
         <v>9</v>
@@ -41283,13 +41283,13 @@
         <v>8</v>
       </c>
       <c r="W18">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="X18">
         <v>7</v>
       </c>
       <c r="Y18">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Z18">
         <v>7</v>
@@ -41351,13 +41351,13 @@
         <v>5</v>
       </c>
       <c r="P19">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Q19">
         <v>6</v>
       </c>
       <c r="R19">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="S19">
         <v>6</v>
@@ -41372,13 +41372,13 @@
         <v>9</v>
       </c>
       <c r="W19">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="X19">
         <v>6</v>
       </c>
       <c r="Y19">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Z19">
         <v>6</v>
@@ -41440,13 +41440,13 @@
         <v>7</v>
       </c>
       <c r="P20">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="Q20">
         <v>6</v>
       </c>
       <c r="R20">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="S20">
         <v>7</v>
@@ -41529,13 +41529,13 @@
         <v>8</v>
       </c>
       <c r="P21">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="Q21">
         <v>6</v>
       </c>
       <c r="R21">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="S21">
         <v>9</v>
@@ -41618,13 +41618,13 @@
         <v>5</v>
       </c>
       <c r="P22">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Q22">
         <v>6</v>
       </c>
       <c r="R22">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="S22">
         <v>7</v>
@@ -41639,13 +41639,13 @@
         <v>8</v>
       </c>
       <c r="W22">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="X22">
         <v>6</v>
       </c>
       <c r="Y22">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Z22">
         <v>6</v>
@@ -41707,13 +41707,13 @@
         <v>6</v>
       </c>
       <c r="P23">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Q23">
         <v>5</v>
       </c>
       <c r="R23">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="S23">
         <v>6</v>
@@ -41728,13 +41728,13 @@
         <v>6</v>
       </c>
       <c r="W23">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="X23">
         <v>6</v>
       </c>
       <c r="Y23">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Z23">
         <v>6</v>
@@ -41796,13 +41796,13 @@
         <v>5</v>
       </c>
       <c r="P24">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Q24">
         <v>5</v>
       </c>
       <c r="R24">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="S24">
         <v>6</v>
@@ -50130,13 +50130,13 @@
         <v>842</v>
       </c>
       <c r="B7">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>5</v>
       </c>
       <c r="D7">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="E7">
         <v>6</v>
@@ -50151,13 +50151,13 @@
         <v>5</v>
       </c>
       <c r="I7">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="J7">
         <v>5</v>
       </c>
       <c r="K7">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="L7">
         <v>-1</v>
@@ -50172,7 +50172,7 @@
         <v>6</v>
       </c>
       <c r="P7">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Q7">
         <v>5</v>
@@ -50193,13 +50193,13 @@
         <v>7</v>
       </c>
       <c r="W7">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="X7">
         <v>5</v>
       </c>
       <c r="Y7">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Z7">
         <v>6</v>
@@ -50335,7 +50335,7 @@
         <v>5</v>
       </c>
       <c r="K9">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="L9">
         <v>-1</v>
@@ -50513,7 +50513,7 @@
         <v>5</v>
       </c>
       <c r="K11">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="L11">
         <v>-1</v>
@@ -50555,7 +50555,7 @@
         <v>5</v>
       </c>
       <c r="Y11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Z11">
         <v>6</v>
@@ -50780,7 +50780,7 @@
         <v>5</v>
       </c>
       <c r="K14">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="L14">
         <v>8</v>
@@ -50822,7 +50822,7 @@
         <v>6</v>
       </c>
       <c r="Y14">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Z14">
         <v>8</v>
@@ -51026,7 +51026,7 @@
         <v>5</v>
       </c>
       <c r="D17">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="E17">
         <v>7</v>
@@ -51047,7 +51047,7 @@
         <v>5</v>
       </c>
       <c r="K17">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="L17">
         <v>-1</v>
@@ -51089,7 +51089,7 @@
         <v>5</v>
       </c>
       <c r="Y17">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Z17">
         <v>7</v>
@@ -51198,13 +51198,13 @@
         <v>854</v>
       </c>
       <c r="B19">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="C19">
         <v>6</v>
       </c>
       <c r="D19">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="E19">
         <v>7</v>
@@ -51219,13 +51219,13 @@
         <v>6</v>
       </c>
       <c r="I19">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="J19">
         <v>5</v>
       </c>
       <c r="K19">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="L19">
         <v>-1</v>
@@ -51240,7 +51240,7 @@
         <v>7</v>
       </c>
       <c r="P19">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Q19">
         <v>7</v>
@@ -51261,13 +51261,13 @@
         <v>7</v>
       </c>
       <c r="W19">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="X19">
         <v>6</v>
       </c>
       <c r="Y19">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="Z19">
         <v>7</v>
@@ -51287,7 +51287,7 @@
         <v>855</v>
       </c>
       <c r="B20">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="C20">
         <v>5</v>
@@ -51308,13 +51308,13 @@
         <v>5</v>
       </c>
       <c r="I20">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="J20">
         <v>5</v>
       </c>
       <c r="K20">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="L20">
         <v>-1</v>
@@ -51329,7 +51329,7 @@
         <v>6</v>
       </c>
       <c r="P20">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Q20">
         <v>5</v>
@@ -51350,7 +51350,7 @@
         <v>7</v>
       </c>
       <c r="W20">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="X20">
         <v>5</v>
@@ -51492,7 +51492,7 @@
         <v>7</v>
       </c>
       <c r="K22">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="L22">
         <v>8</v>
@@ -51670,7 +51670,7 @@
         <v>5</v>
       </c>
       <c r="K24">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="L24">
         <v>7</v>
@@ -51712,7 +51712,7 @@
         <v>6</v>
       </c>
       <c r="Y24">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="Z24">
         <v>7</v>
@@ -52026,7 +52026,7 @@
         <v>5</v>
       </c>
       <c r="K28">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="L28">
         <v>6</v>
@@ -52068,7 +52068,7 @@
         <v>7</v>
       </c>
       <c r="Y28">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Z28">
         <v>7</v>
@@ -52649,7 +52649,7 @@
         <v>5</v>
       </c>
       <c r="K35">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="L35">
         <v>9</v>
@@ -52691,7 +52691,7 @@
         <v>6</v>
       </c>
       <c r="Y35">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Z35">
         <v>8</v>
@@ -53047,7 +53047,7 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -53068,7 +53068,7 @@
         <v>5</v>
       </c>
       <c r="J5">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="K5">
         <v>6</v>
@@ -53089,7 +53089,7 @@
         <v>7</v>
       </c>
       <c r="Q5">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="R5">
         <v>7</v>
@@ -53110,7 +53110,7 @@
         <v>6</v>
       </c>
       <c r="X5">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Y5">
         <v>6</v>
@@ -53225,7 +53225,7 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>7</v>
@@ -53246,7 +53246,7 @@
         <v>5</v>
       </c>
       <c r="J7">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="K7">
         <v>7</v>
@@ -53267,7 +53267,7 @@
         <v>7</v>
       </c>
       <c r="Q7">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="R7">
         <v>7</v>
@@ -53288,7 +53288,7 @@
         <v>6</v>
       </c>
       <c r="X7">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Y7">
         <v>7</v>
@@ -53492,7 +53492,7 @@
         <v>6</v>
       </c>
       <c r="C10">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D10">
         <v>6</v>
@@ -53513,7 +53513,7 @@
         <v>5</v>
       </c>
       <c r="J10">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="K10">
         <v>6</v>
@@ -53534,7 +53534,7 @@
         <v>7</v>
       </c>
       <c r="Q10">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="R10">
         <v>6</v>
@@ -53555,7 +53555,7 @@
         <v>6</v>
       </c>
       <c r="X10">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Y10">
         <v>6</v>
@@ -54115,7 +54115,7 @@
         <v>6</v>
       </c>
       <c r="C17">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D17">
         <v>5</v>
@@ -54136,7 +54136,7 @@
         <v>5</v>
       </c>
       <c r="J17">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="K17">
         <v>5</v>
@@ -54157,7 +54157,7 @@
         <v>7</v>
       </c>
       <c r="Q17">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="R17">
         <v>8</v>
@@ -54178,7 +54178,7 @@
         <v>6</v>
       </c>
       <c r="X17">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Y17">
         <v>6</v>
@@ -54204,7 +54204,7 @@
         <v>6</v>
       </c>
       <c r="C18">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D18">
         <v>5</v>
@@ -54225,7 +54225,7 @@
         <v>5</v>
       </c>
       <c r="J18">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="K18">
         <v>5</v>
@@ -54246,7 +54246,7 @@
         <v>7</v>
       </c>
       <c r="Q18">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="R18">
         <v>8</v>
@@ -54267,7 +54267,7 @@
         <v>6</v>
       </c>
       <c r="X18">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Y18">
         <v>6</v>
@@ -54649,7 +54649,7 @@
         <v>8</v>
       </c>
       <c r="C23">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D23">
         <v>7</v>
@@ -54670,7 +54670,7 @@
         <v>5</v>
       </c>
       <c r="J23">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="K23">
         <v>6</v>
@@ -54691,7 +54691,7 @@
         <v>7</v>
       </c>
       <c r="Q23">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="R23">
         <v>6</v>
@@ -54712,7 +54712,7 @@
         <v>7</v>
       </c>
       <c r="X23">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Y23">
         <v>6</v>
@@ -54827,7 +54827,7 @@
         <v>6</v>
       </c>
       <c r="C25">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D25">
         <v>5</v>
@@ -54848,7 +54848,7 @@
         <v>6</v>
       </c>
       <c r="J25">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="K25">
         <v>6</v>
@@ -54869,7 +54869,7 @@
         <v>7</v>
       </c>
       <c r="Q25">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="R25">
         <v>7</v>
@@ -54890,7 +54890,7 @@
         <v>6</v>
       </c>
       <c r="X25">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Y25">
         <v>6</v>
@@ -54916,7 +54916,7 @@
         <v>6</v>
       </c>
       <c r="C26">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D26">
         <v>6</v>
@@ -54937,7 +54937,7 @@
         <v>5</v>
       </c>
       <c r="J26">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="K26">
         <v>6</v>
@@ -54958,7 +54958,7 @@
         <v>7</v>
       </c>
       <c r="Q26">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="R26">
         <v>6</v>
@@ -54979,7 +54979,7 @@
         <v>6</v>
       </c>
       <c r="X26">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Y26">
         <v>6</v>
@@ -55005,13 +55005,13 @@
         <v>6</v>
       </c>
       <c r="C27">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D27">
         <v>5</v>
       </c>
       <c r="E27">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="F27">
         <v>-1</v>
@@ -55026,13 +55026,13 @@
         <v>5</v>
       </c>
       <c r="J27">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="K27">
         <v>6</v>
       </c>
       <c r="L27">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="M27">
         <v>-1</v>
@@ -55047,13 +55047,13 @@
         <v>7</v>
       </c>
       <c r="Q27">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="R27">
         <v>7</v>
       </c>
       <c r="S27">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="T27">
         <v>-1</v>
@@ -55068,13 +55068,13 @@
         <v>6</v>
       </c>
       <c r="X27">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Y27">
         <v>6</v>
       </c>
       <c r="Z27">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="AA27">
         <v>-1</v>
@@ -55094,13 +55094,13 @@
         <v>6</v>
       </c>
       <c r="C28">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D28">
         <v>5</v>
       </c>
       <c r="E28">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="F28">
         <v>-1</v>
@@ -55115,13 +55115,13 @@
         <v>6</v>
       </c>
       <c r="J28">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="K28">
         <v>6</v>
       </c>
       <c r="L28">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="M28">
         <v>-1</v>
@@ -55136,13 +55136,13 @@
         <v>7</v>
       </c>
       <c r="Q28">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="R28">
         <v>7</v>
       </c>
       <c r="S28">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="T28">
         <v>-1</v>
@@ -55157,13 +55157,13 @@
         <v>6</v>
       </c>
       <c r="X28">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Y28">
         <v>6</v>
       </c>
       <c r="Z28">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="AA28">
         <v>-1</v>
@@ -55272,13 +55272,13 @@
         <v>6</v>
       </c>
       <c r="C30">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D30">
         <v>8</v>
       </c>
       <c r="E30">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="F30">
         <v>-1</v>
@@ -55293,13 +55293,13 @@
         <v>6</v>
       </c>
       <c r="J30">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="K30">
         <v>8</v>
       </c>
       <c r="L30">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="M30">
         <v>-1</v>
@@ -55314,13 +55314,13 @@
         <v>7</v>
       </c>
       <c r="Q30">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="R30">
         <v>7</v>
       </c>
       <c r="S30">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="T30">
         <v>-1</v>
@@ -55335,13 +55335,13 @@
         <v>6</v>
       </c>
       <c r="X30">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Y30">
         <v>8</v>
       </c>
       <c r="Z30">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="AA30">
         <v>-1</v>
@@ -55717,7 +55717,7 @@
         <v>6</v>
       </c>
       <c r="C35">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D35">
         <v>5</v>
@@ -55738,7 +55738,7 @@
         <v>5</v>
       </c>
       <c r="J35">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="K35">
         <v>6</v>
@@ -55759,7 +55759,7 @@
         <v>7</v>
       </c>
       <c r="Q35">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="R35">
         <v>7</v>
@@ -55780,7 +55780,7 @@
         <v>6</v>
       </c>
       <c r="X35">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Y35">
         <v>6</v>
@@ -55806,7 +55806,7 @@
         <v>6</v>
       </c>
       <c r="C36">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D36">
         <v>7</v>
@@ -55827,7 +55827,7 @@
         <v>6</v>
       </c>
       <c r="J36">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="K36">
         <v>8</v>
@@ -55848,7 +55848,7 @@
         <v>7</v>
       </c>
       <c r="Q36">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="R36">
         <v>7</v>
@@ -55869,7 +55869,7 @@
         <v>6</v>
       </c>
       <c r="X36">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Y36">
         <v>7</v>
@@ -55984,13 +55984,13 @@
         <v>6</v>
       </c>
       <c r="C38">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D38">
         <v>5</v>
       </c>
       <c r="E38">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="F38">
         <v>-1</v>
@@ -56005,13 +56005,13 @@
         <v>5</v>
       </c>
       <c r="J38">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="K38">
         <v>6</v>
       </c>
       <c r="L38">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="M38">
         <v>-1</v>
@@ -56026,13 +56026,13 @@
         <v>7</v>
       </c>
       <c r="Q38">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="R38">
         <v>7</v>
       </c>
       <c r="S38">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="T38">
         <v>-1</v>
@@ -56047,13 +56047,13 @@
         <v>6</v>
       </c>
       <c r="X38">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Y38">
         <v>6</v>
       </c>
       <c r="Z38">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="AA38">
         <v>-1</v>
@@ -56073,7 +56073,7 @@
         <v>6</v>
       </c>
       <c r="C39">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D39">
         <v>6</v>
@@ -56094,7 +56094,7 @@
         <v>5</v>
       </c>
       <c r="J39">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="K39">
         <v>6</v>
@@ -56115,7 +56115,7 @@
         <v>7</v>
       </c>
       <c r="Q39">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="R39">
         <v>6</v>
@@ -56136,7 +56136,7 @@
         <v>6</v>
       </c>
       <c r="X39">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Y39">
         <v>6</v>
@@ -56162,7 +56162,7 @@
         <v>6</v>
       </c>
       <c r="C40">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D40">
         <v>8</v>
@@ -56183,7 +56183,7 @@
         <v>6</v>
       </c>
       <c r="J40">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="K40">
         <v>8</v>
@@ -56204,7 +56204,7 @@
         <v>7</v>
       </c>
       <c r="Q40">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="R40">
         <v>8</v>
@@ -56225,7 +56225,7 @@
         <v>6</v>
       </c>
       <c r="X40">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Y40">
         <v>8</v>
@@ -56251,7 +56251,7 @@
         <v>9</v>
       </c>
       <c r="C41">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D41">
         <v>7</v>
@@ -56272,7 +56272,7 @@
         <v>6</v>
       </c>
       <c r="J41">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="K41">
         <v>8</v>
@@ -56293,7 +56293,7 @@
         <v>7</v>
       </c>
       <c r="Q41">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="R41">
         <v>7</v>
@@ -56314,7 +56314,7 @@
         <v>7</v>
       </c>
       <c r="X41">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Y41">
         <v>7</v>
@@ -57752,7 +57752,7 @@
         <v>6</v>
       </c>
       <c r="C20">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D20">
         <v>5</v>
@@ -57770,7 +57770,7 @@
         <v>6</v>
       </c>
       <c r="I20">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="J20">
         <v>5</v>
@@ -57788,7 +57788,7 @@
         <v>6</v>
       </c>
       <c r="O20">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="P20">
         <v>8</v>
@@ -57806,7 +57806,7 @@
         <v>6</v>
       </c>
       <c r="U20">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="V20">
         <v>6</v>
@@ -58522,7 +58522,7 @@
         <v>8</v>
       </c>
       <c r="C30">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D30">
         <v>5</v>
@@ -58540,7 +58540,7 @@
         <v>5</v>
       </c>
       <c r="I30">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="J30">
         <v>5</v>
@@ -58558,7 +58558,7 @@
         <v>5</v>
       </c>
       <c r="O30">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="P30">
         <v>5</v>
@@ -58576,7 +58576,7 @@
         <v>6</v>
       </c>
       <c r="U30">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="V30">
         <v>5</v>
@@ -59292,7 +59292,7 @@
         <v>6</v>
       </c>
       <c r="C40">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D40">
         <v>5</v>
@@ -59310,7 +59310,7 @@
         <v>5</v>
       </c>
       <c r="I40">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="J40">
         <v>5</v>
@@ -59328,7 +59328,7 @@
         <v>7</v>
       </c>
       <c r="O40">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="P40">
         <v>5</v>
@@ -59346,7 +59346,7 @@
         <v>6</v>
       </c>
       <c r="U40">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="V40">
         <v>5</v>
@@ -59742,7 +59742,7 @@
         <v>6</v>
       </c>
       <c r="D5">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="E5">
         <v>-1</v>
@@ -59760,7 +59760,7 @@
         <v>6</v>
       </c>
       <c r="J5">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="K5">
         <v>-1</v>
@@ -59778,7 +59778,7 @@
         <v>8</v>
       </c>
       <c r="P5">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Q5">
         <v>-1</v>
@@ -59796,7 +59796,7 @@
         <v>7</v>
       </c>
       <c r="V5">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="W5">
         <v>-1</v>
@@ -60079,7 +60079,7 @@
         <v>9</v>
       </c>
       <c r="D10">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="E10">
         <v>9</v>
@@ -60097,7 +60097,7 @@
         <v>8</v>
       </c>
       <c r="J10">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="K10">
         <v>-1</v>
@@ -60115,7 +60115,7 @@
         <v>8</v>
       </c>
       <c r="P10">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Q10">
         <v>-1</v>
@@ -60133,7 +60133,7 @@
         <v>8</v>
       </c>
       <c r="V10">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="W10">
         <v>9</v>
@@ -60156,7 +60156,7 @@
         <v>5</v>
       </c>
       <c r="D11">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="E11">
         <v>-1</v>
@@ -60174,7 +60174,7 @@
         <v>5</v>
       </c>
       <c r="J11">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="K11">
         <v>-1</v>
@@ -60192,7 +60192,7 @@
         <v>8</v>
       </c>
       <c r="P11">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Q11">
         <v>-1</v>
@@ -60210,7 +60210,7 @@
         <v>6</v>
       </c>
       <c r="V11">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="W11">
         <v>-1</v>
@@ -60926,7 +60926,7 @@
         <v>5</v>
       </c>
       <c r="D21">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="E21">
         <v>-1</v>
@@ -60944,7 +60944,7 @@
         <v>5</v>
       </c>
       <c r="J21">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="K21">
         <v>-1</v>
@@ -60962,7 +60962,7 @@
         <v>8</v>
       </c>
       <c r="P21">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Q21">
         <v>-1</v>
@@ -60980,7 +60980,7 @@
         <v>6</v>
       </c>
       <c r="V21">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="W21">
         <v>-1</v>
@@ -61157,7 +61157,7 @@
         <v>5</v>
       </c>
       <c r="D24">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="E24">
         <v>-1</v>
@@ -61175,7 +61175,7 @@
         <v>5</v>
       </c>
       <c r="J24">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="K24">
         <v>-1</v>
@@ -61193,7 +61193,7 @@
         <v>8</v>
       </c>
       <c r="P24">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Q24">
         <v>-1</v>
@@ -61211,7 +61211,7 @@
         <v>6</v>
       </c>
       <c r="V24">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="W24">
         <v>-1</v>
@@ -61956,7 +61956,7 @@
         <v>5</v>
       </c>
       <c r="D35">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="E35">
         <v>-1</v>
@@ -61974,7 +61974,7 @@
         <v>5</v>
       </c>
       <c r="J35">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="K35">
         <v>-1</v>
@@ -61992,7 +61992,7 @@
         <v>8</v>
       </c>
       <c r="P35">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Q35">
         <v>-1</v>
@@ -62010,7 +62010,7 @@
         <v>6</v>
       </c>
       <c r="V35">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="W35">
         <v>-1</v>
@@ -62033,7 +62033,7 @@
         <v>8</v>
       </c>
       <c r="D36">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="E36">
         <v>-1</v>
@@ -62051,7 +62051,7 @@
         <v>5</v>
       </c>
       <c r="J36">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="K36">
         <v>-1</v>
@@ -62069,7 +62069,7 @@
         <v>8</v>
       </c>
       <c r="P36">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Q36">
         <v>-1</v>
@@ -62087,7 +62087,7 @@
         <v>7</v>
       </c>
       <c r="V36">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="W36">
         <v>-1</v>
@@ -62110,7 +62110,7 @@
         <v>6</v>
       </c>
       <c r="D37">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="E37">
         <v>-1</v>
@@ -62128,7 +62128,7 @@
         <v>7</v>
       </c>
       <c r="J37">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="K37">
         <v>-1</v>
@@ -62146,7 +62146,7 @@
         <v>8</v>
       </c>
       <c r="P37">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Q37">
         <v>-1</v>
@@ -62164,7 +62164,7 @@
         <v>7</v>
       </c>
       <c r="V37">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="W37">
         <v>-1</v>
@@ -62187,7 +62187,7 @@
         <v>6</v>
       </c>
       <c r="D38">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="E38">
         <v>-1</v>
@@ -62205,7 +62205,7 @@
         <v>6</v>
       </c>
       <c r="J38">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="K38">
         <v>-1</v>
@@ -62223,7 +62223,7 @@
         <v>8</v>
       </c>
       <c r="P38">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Q38">
         <v>-1</v>
@@ -62241,7 +62241,7 @@
         <v>7</v>
       </c>
       <c r="V38">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="W38">
         <v>-1</v>
@@ -69320,7 +69320,7 @@
         <v>6</v>
       </c>
       <c r="L4">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="M4">
         <v>-1</v>
@@ -69338,7 +69338,7 @@
         <v>6</v>
       </c>
       <c r="R4">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="S4">
         <v>-1</v>
@@ -70294,7 +70294,7 @@
         <v>6</v>
       </c>
       <c r="C17">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="D17">
         <v>5</v>
@@ -70312,7 +70312,7 @@
         <v>6</v>
       </c>
       <c r="I17">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="J17">
         <v>5</v>
@@ -70330,7 +70330,7 @@
         <v>7</v>
       </c>
       <c r="O17">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="P17">
         <v>-1</v>
@@ -70339,7 +70339,7 @@
         <v>6</v>
       </c>
       <c r="R17">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="S17">
         <v>-1</v>
@@ -70348,7 +70348,7 @@
         <v>6</v>
       </c>
       <c r="U17">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="V17">
         <v>5</v>
@@ -70357,7 +70357,7 @@
         <v>6</v>
       </c>
       <c r="X17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Y17">
         <v>-1</v>
@@ -70679,7 +70679,7 @@
         <v>5</v>
       </c>
       <c r="C22">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D22">
         <v>5</v>
@@ -70697,7 +70697,7 @@
         <v>6</v>
       </c>
       <c r="I22">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="J22">
         <v>5</v>
@@ -70715,7 +70715,7 @@
         <v>7</v>
       </c>
       <c r="O22">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="P22">
         <v>-1</v>
@@ -70733,7 +70733,7 @@
         <v>6</v>
       </c>
       <c r="U22">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="V22">
         <v>5</v>
@@ -81109,7 +81109,7 @@
         <v>9</v>
       </c>
       <c r="N4">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="O4">
         <v>-1</v>
@@ -81186,7 +81186,7 @@
         <v>10</v>
       </c>
       <c r="N5">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="O5">
         <v>-1</v>
@@ -81263,7 +81263,7 @@
         <v>5</v>
       </c>
       <c r="N6">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="O6">
         <v>-1</v>
@@ -81281,7 +81281,7 @@
         <v>8</v>
       </c>
       <c r="T6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="U6">
         <v>6</v>
@@ -81340,7 +81340,7 @@
         <v>5</v>
       </c>
       <c r="N7">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="O7">
         <v>-1</v>
@@ -81417,7 +81417,7 @@
         <v>9</v>
       </c>
       <c r="N8">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="O8">
         <v>-1</v>
@@ -81494,7 +81494,7 @@
         <v>5</v>
       </c>
       <c r="N9">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="O9">
         <v>-1</v>
@@ -81571,7 +81571,7 @@
         <v>10</v>
       </c>
       <c r="N10">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="O10">
         <v>-1</v>
@@ -81648,7 +81648,7 @@
         <v>10</v>
       </c>
       <c r="N11">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="O11">
         <v>-1</v>
@@ -81725,7 +81725,7 @@
         <v>5</v>
       </c>
       <c r="N12">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="O12">
         <v>-1</v>
@@ -81802,7 +81802,7 @@
         <v>10</v>
       </c>
       <c r="N13">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="O13">
         <v>-1</v>
@@ -81879,7 +81879,7 @@
         <v>5</v>
       </c>
       <c r="N14">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="O14">
         <v>-1</v>
@@ -81956,7 +81956,7 @@
         <v>10</v>
       </c>
       <c r="N15">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="O15">
         <v>-1</v>
@@ -82033,7 +82033,7 @@
         <v>10</v>
       </c>
       <c r="N16">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="O16">
         <v>-1</v>
@@ -82110,7 +82110,7 @@
         <v>9</v>
       </c>
       <c r="N17">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="O17">
         <v>-1</v>
@@ -82187,7 +82187,7 @@
         <v>10</v>
       </c>
       <c r="N18">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="O18">
         <v>-1</v>
@@ -82205,7 +82205,7 @@
         <v>9</v>
       </c>
       <c r="T18">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="U18">
         <v>9</v>
@@ -82264,7 +82264,7 @@
         <v>6</v>
       </c>
       <c r="N19">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="O19">
         <v>-1</v>
@@ -82341,7 +82341,7 @@
         <v>10</v>
       </c>
       <c r="N20">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="O20">
         <v>-1</v>
@@ -82359,7 +82359,7 @@
         <v>8</v>
       </c>
       <c r="T20">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="U20">
         <v>9</v>
@@ -82418,7 +82418,7 @@
         <v>5</v>
       </c>
       <c r="N21">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="O21">
         <v>-1</v>
@@ -82433,10 +82433,10 @@
         <v>-1</v>
       </c>
       <c r="S21">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="T21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="U21">
         <v>5</v>
@@ -82451,7 +82451,7 @@
         <v>7</v>
       </c>
       <c r="Y21">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:25">
@@ -82495,7 +82495,7 @@
         <v>5</v>
       </c>
       <c r="N22">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="O22">
         <v>-1</v>
@@ -82513,7 +82513,7 @@
         <v>5</v>
       </c>
       <c r="T22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="U22">
         <v>5</v>
@@ -82572,7 +82572,7 @@
         <v>6</v>
       </c>
       <c r="N23">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="O23">
         <v>-1</v>
@@ -82649,7 +82649,7 @@
         <v>6</v>
       </c>
       <c r="N24">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="O24">
         <v>-1</v>
@@ -82664,10 +82664,10 @@
         <v>-1</v>
       </c>
       <c r="S24">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="T24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="U24">
         <v>5</v>
@@ -82682,7 +82682,7 @@
         <v>-1</v>
       </c>
       <c r="Y24">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:25">
@@ -82726,7 +82726,7 @@
         <v>9</v>
       </c>
       <c r="N25">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="O25">
         <v>-1</v>
@@ -82803,7 +82803,7 @@
         <v>5</v>
       </c>
       <c r="N26">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="O26">
         <v>-1</v>
@@ -82880,7 +82880,7 @@
         <v>5</v>
       </c>
       <c r="N27">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="O27">
         <v>-1</v>
@@ -82898,7 +82898,7 @@
         <v>5</v>
       </c>
       <c r="T27">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="U27">
         <v>5</v>
@@ -82957,7 +82957,7 @@
         <v>9</v>
       </c>
       <c r="N28">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="O28">
         <v>-1</v>
@@ -82975,7 +82975,7 @@
         <v>6</v>
       </c>
       <c r="T28">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U28">
         <v>9</v>
@@ -83034,7 +83034,7 @@
         <v>5</v>
       </c>
       <c r="N29">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="O29">
         <v>-1</v>
@@ -83049,7 +83049,7 @@
         <v>-1</v>
       </c>
       <c r="S29">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="T29">
         <v>6</v>
@@ -83067,7 +83067,7 @@
         <v>7</v>
       </c>
       <c r="Y29">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:25">
@@ -83111,7 +83111,7 @@
         <v>5</v>
       </c>
       <c r="N30">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="O30">
         <v>-1</v>
@@ -83126,10 +83126,10 @@
         <v>-1</v>
       </c>
       <c r="S30">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="T30">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="U30">
         <v>6</v>
@@ -83144,7 +83144,7 @@
         <v>-1</v>
       </c>
       <c r="Y30">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:25">
@@ -83188,7 +83188,7 @@
         <v>9</v>
       </c>
       <c r="N31">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="O31">
         <v>-1</v>
@@ -83206,7 +83206,7 @@
         <v>8</v>
       </c>
       <c r="T31">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U31">
         <v>9</v>
@@ -83265,7 +83265,7 @@
         <v>6</v>
       </c>
       <c r="N32">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="O32">
         <v>-1</v>
@@ -83342,7 +83342,7 @@
         <v>5</v>
       </c>
       <c r="N33">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="O33">
         <v>-1</v>
@@ -83419,7 +83419,7 @@
         <v>10</v>
       </c>
       <c r="N34">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="O34">
         <v>-1</v>
@@ -83496,7 +83496,7 @@
         <v>10</v>
       </c>
       <c r="N35">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="O35">
         <v>-1</v>
@@ -83573,7 +83573,7 @@
         <v>5</v>
       </c>
       <c r="N36">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="O36">
         <v>-1</v>
@@ -83591,7 +83591,7 @@
         <v>9</v>
       </c>
       <c r="T36">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="U36">
         <v>5</v>
@@ -83650,7 +83650,7 @@
         <v>6</v>
       </c>
       <c r="N37">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="O37">
         <v>-1</v>
@@ -83727,7 +83727,7 @@
         <v>10</v>
       </c>
       <c r="N38">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="O38">
         <v>-1</v>
@@ -83804,7 +83804,7 @@
         <v>10</v>
       </c>
       <c r="N39">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="O39">
         <v>-1</v>

</xml_diff>

<commit_message>
Actualizacion Datos Personales 4 nov
</commit_message>
<xml_diff>
--- a/Calificaciones.xlsx
+++ b/Calificaciones.xlsx
@@ -6832,7 +6832,7 @@
         <v>7</v>
       </c>
       <c r="G6">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="H6">
         <v>-1</v>
@@ -6886,7 +6886,7 @@
         <v>7</v>
       </c>
       <c r="Y6">
-        <v>-1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -7371,7 +7371,7 @@
         <v>6</v>
       </c>
       <c r="G13">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="H13">
         <v>-1</v>
@@ -7425,7 +7425,7 @@
         <v>6</v>
       </c>
       <c r="Y13">
-        <v>-1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -7833,7 +7833,7 @@
         <v>6</v>
       </c>
       <c r="G19">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="H19">
         <v>-1</v>
@@ -7887,7 +7887,7 @@
         <v>6</v>
       </c>
       <c r="Y19">
-        <v>-1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:25">
@@ -8526,7 +8526,7 @@
         <v>9</v>
       </c>
       <c r="G28">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="H28">
         <v>-1</v>
@@ -8580,7 +8580,7 @@
         <v>9</v>
       </c>
       <c r="Y28">
-        <v>-1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:25">
@@ -9219,7 +9219,7 @@
         <v>6</v>
       </c>
       <c r="G37">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="H37">
         <v>-1</v>
@@ -9273,7 +9273,7 @@
         <v>6</v>
       </c>
       <c r="Y37">
-        <v>-1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:25">
@@ -18557,7 +18557,7 @@
         <v>6</v>
       </c>
       <c r="E5">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="F5">
         <v>7</v>
@@ -18611,7 +18611,7 @@
         <v>6</v>
       </c>
       <c r="W5">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="X5">
         <v>7</v>
@@ -18711,7 +18711,7 @@
         <v>-1</v>
       </c>
       <c r="E7">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="F7">
         <v>8</v>
@@ -18765,7 +18765,7 @@
         <v>-1</v>
       </c>
       <c r="W7">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="X7">
         <v>8</v>
@@ -18942,7 +18942,7 @@
         <v>8</v>
       </c>
       <c r="E10">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="F10">
         <v>-1</v>
@@ -18996,7 +18996,7 @@
         <v>8</v>
       </c>
       <c r="W10">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="X10">
         <v>-1</v>
@@ -19096,7 +19096,7 @@
         <v>-1</v>
       </c>
       <c r="E12">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="F12">
         <v>7</v>
@@ -19150,7 +19150,7 @@
         <v>-1</v>
       </c>
       <c r="W12">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="X12">
         <v>7</v>
@@ -19250,7 +19250,7 @@
         <v>-1</v>
       </c>
       <c r="E14">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="F14">
         <v>-1</v>
@@ -19304,7 +19304,7 @@
         <v>-1</v>
       </c>
       <c r="W14">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="X14">
         <v>-1</v>
@@ -19866,7 +19866,7 @@
         <v>8</v>
       </c>
       <c r="E22">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="F22">
         <v>-1</v>
@@ -19920,7 +19920,7 @@
         <v>8</v>
       </c>
       <c r="W22">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="X22">
         <v>-1</v>
@@ -20097,7 +20097,7 @@
         <v>-1</v>
       </c>
       <c r="E25">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="F25">
         <v>-1</v>
@@ -20151,7 +20151,7 @@
         <v>-1</v>
       </c>
       <c r="W25">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="X25">
         <v>-1</v>
@@ -20790,7 +20790,7 @@
         <v>-1</v>
       </c>
       <c r="E34">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="F34">
         <v>-1</v>
@@ -20844,7 +20844,7 @@
         <v>-1</v>
       </c>
       <c r="W34">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="X34">
         <v>-1</v>
@@ -21098,7 +21098,7 @@
         <v>7</v>
       </c>
       <c r="E38">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="F38">
         <v>-1</v>
@@ -21152,7 +21152,7 @@
         <v>7</v>
       </c>
       <c r="W38">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="X38">
         <v>-1</v>
@@ -21471,7 +21471,7 @@
         <v>-1</v>
       </c>
       <c r="F6">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="G6">
         <v>7</v>
@@ -21525,7 +21525,7 @@
         <v>-1</v>
       </c>
       <c r="X6">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="Y6">
         <v>7</v>
@@ -21702,7 +21702,7 @@
         <v>7</v>
       </c>
       <c r="F9">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="G9">
         <v>9</v>
@@ -21756,7 +21756,7 @@
         <v>7</v>
       </c>
       <c r="X9">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Y9">
         <v>9</v>
@@ -22010,7 +22010,7 @@
         <v>-1</v>
       </c>
       <c r="F13">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="G13">
         <v>5</v>
@@ -22064,7 +22064,7 @@
         <v>-1</v>
       </c>
       <c r="X13">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="Y13">
         <v>5</v>
@@ -22164,7 +22164,7 @@
         <v>6</v>
       </c>
       <c r="F15">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="G15">
         <v>5</v>
@@ -22218,7 +22218,7 @@
         <v>6</v>
       </c>
       <c r="X15">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="Y15">
         <v>5</v>
@@ -22318,7 +22318,7 @@
         <v>6</v>
       </c>
       <c r="F17">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="G17">
         <v>6</v>
@@ -22372,7 +22372,7 @@
         <v>6</v>
       </c>
       <c r="X17">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Y17">
         <v>6</v>
@@ -22395,7 +22395,7 @@
         <v>6</v>
       </c>
       <c r="F18">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="G18">
         <v>6</v>
@@ -22449,7 +22449,7 @@
         <v>6</v>
       </c>
       <c r="X18">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="Y18">
         <v>6</v>
@@ -22934,7 +22934,7 @@
         <v>-1</v>
       </c>
       <c r="F25">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="G25">
         <v>6</v>
@@ -22988,7 +22988,7 @@
         <v>-1</v>
       </c>
       <c r="X25">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="Y25">
         <v>6</v>
@@ -23088,7 +23088,7 @@
         <v>-1</v>
       </c>
       <c r="F27">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="G27">
         <v>5</v>
@@ -23142,7 +23142,7 @@
         <v>-1</v>
       </c>
       <c r="X27">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="Y27">
         <v>5</v>
@@ -23165,7 +23165,7 @@
         <v>6</v>
       </c>
       <c r="F28">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="G28">
         <v>6</v>
@@ -23219,7 +23219,7 @@
         <v>6</v>
       </c>
       <c r="X28">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="Y28">
         <v>6</v>
@@ -24992,7 +24992,7 @@
         <v>-1</v>
       </c>
       <c r="D24">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="E24">
         <v>-1</v>
@@ -25046,7 +25046,7 @@
         <v>-1</v>
       </c>
       <c r="V24">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="W24">
         <v>-1</v>
@@ -25470,7 +25470,7 @@
         <v>-1</v>
       </c>
       <c r="E5">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="F5">
         <v>10</v>
@@ -25533,7 +25533,7 @@
         <v>-1</v>
       </c>
       <c r="Z5">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="AA5">
         <v>10</v>
@@ -26004,7 +26004,7 @@
         <v>8</v>
       </c>
       <c r="E11">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="F11">
         <v>10</v>
@@ -26067,7 +26067,7 @@
         <v>8</v>
       </c>
       <c r="Z11">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="AA11">
         <v>10</v>
@@ -26093,7 +26093,7 @@
         <v>-1</v>
       </c>
       <c r="E12">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="F12">
         <v>-1</v>
@@ -26156,7 +26156,7 @@
         <v>-1</v>
       </c>
       <c r="Z12">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="AA12">
         <v>-1</v>
@@ -26182,7 +26182,7 @@
         <v>-1</v>
       </c>
       <c r="E13">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="F13">
         <v>-1</v>
@@ -26245,7 +26245,7 @@
         <v>-1</v>
       </c>
       <c r="Z13">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="AA13">
         <v>-1</v>
@@ -26627,7 +26627,7 @@
         <v>-1</v>
       </c>
       <c r="E18">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="F18">
         <v>10</v>
@@ -26690,7 +26690,7 @@
         <v>-1</v>
       </c>
       <c r="Z18">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="AA18">
         <v>10</v>
@@ -26894,7 +26894,7 @@
         <v>7</v>
       </c>
       <c r="E21">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="F21">
         <v>9</v>
@@ -26957,7 +26957,7 @@
         <v>7</v>
       </c>
       <c r="Z21">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="AA21">
         <v>9</v>
@@ -27339,7 +27339,7 @@
         <v>-1</v>
       </c>
       <c r="E26">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="F26">
         <v>8</v>
@@ -27402,7 +27402,7 @@
         <v>-1</v>
       </c>
       <c r="Z26">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="AA26">
         <v>8</v>
@@ -27428,7 +27428,7 @@
         <v>-1</v>
       </c>
       <c r="E27">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="F27">
         <v>-1</v>
@@ -27491,7 +27491,7 @@
         <v>-1</v>
       </c>
       <c r="Z27">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="AA27">
         <v>-1</v>
@@ -27606,7 +27606,7 @@
         <v>8</v>
       </c>
       <c r="E29">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="F29">
         <v>-1</v>
@@ -27669,7 +27669,7 @@
         <v>8</v>
       </c>
       <c r="Z29">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="AA29">
         <v>-1</v>
@@ -27784,7 +27784,7 @@
         <v>7</v>
       </c>
       <c r="E31">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="F31">
         <v>10</v>
@@ -27847,7 +27847,7 @@
         <v>7</v>
       </c>
       <c r="Z31">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="AA31">
         <v>10</v>
@@ -27873,7 +27873,7 @@
         <v>7</v>
       </c>
       <c r="E32">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="F32">
         <v>10</v>
@@ -27936,7 +27936,7 @@
         <v>7</v>
       </c>
       <c r="Z32">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="AA32">
         <v>10</v>
@@ -28984,7 +28984,7 @@
         <v>8</v>
       </c>
       <c r="E12">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="F12">
         <v>-1</v>
@@ -29038,7 +29038,7 @@
         <v>8</v>
       </c>
       <c r="W12">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="X12">
         <v>-1</v>
@@ -29446,7 +29446,7 @@
         <v>8</v>
       </c>
       <c r="E18">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="F18">
         <v>8</v>
@@ -29500,7 +29500,7 @@
         <v>8</v>
       </c>
       <c r="W18">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="X18">
         <v>8</v>
@@ -29600,7 +29600,7 @@
         <v>8</v>
       </c>
       <c r="E20">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="F20">
         <v>7</v>
@@ -29654,7 +29654,7 @@
         <v>8</v>
       </c>
       <c r="W20">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="X20">
         <v>7</v>
@@ -29831,7 +29831,7 @@
         <v>8</v>
       </c>
       <c r="E23">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="F23">
         <v>-1</v>
@@ -29885,7 +29885,7 @@
         <v>8</v>
       </c>
       <c r="W23">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="X23">
         <v>-1</v>
@@ -30216,7 +30216,7 @@
         <v>7</v>
       </c>
       <c r="E28">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="F28">
         <v>-1</v>
@@ -30270,7 +30270,7 @@
         <v>7</v>
       </c>
       <c r="W28">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="X28">
         <v>-1</v>
@@ -30293,7 +30293,7 @@
         <v>7</v>
       </c>
       <c r="E29">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="F29">
         <v>7</v>
@@ -30347,7 +30347,7 @@
         <v>7</v>
       </c>
       <c r="W29">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="X29">
         <v>7</v>
@@ -30447,7 +30447,7 @@
         <v>-1</v>
       </c>
       <c r="E31">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="F31">
         <v>-1</v>
@@ -30501,7 +30501,7 @@
         <v>-1</v>
       </c>
       <c r="W31">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="X31">
         <v>-1</v>
@@ -31581,7 +31581,7 @@
         <v>6</v>
       </c>
       <c r="C10">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D10">
         <v>6</v>
@@ -31635,7 +31635,7 @@
         <v>6</v>
       </c>
       <c r="U10">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="V10">
         <v>6</v>
@@ -31889,7 +31889,7 @@
         <v>-1</v>
       </c>
       <c r="C14">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D14">
         <v>-1</v>
@@ -31943,7 +31943,7 @@
         <v>-1</v>
       </c>
       <c r="U14">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="V14">
         <v>-1</v>
@@ -32052,7 +32052,7 @@
         <v>-1</v>
       </c>
       <c r="F16">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="G16">
         <v>-1</v>
@@ -32106,7 +32106,7 @@
         <v>-1</v>
       </c>
       <c r="X16">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="Y16">
         <v>-1</v>
@@ -32428,7 +32428,7 @@
         <v>-1</v>
       </c>
       <c r="C21">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D21">
         <v>-1</v>
@@ -32482,7 +32482,7 @@
         <v>-1</v>
       </c>
       <c r="U21">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="V21">
         <v>-1</v>
@@ -32582,7 +32582,7 @@
         <v>-1</v>
       </c>
       <c r="C23">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D23">
         <v>-1</v>
@@ -32636,7 +32636,7 @@
         <v>-1</v>
       </c>
       <c r="U23">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="V23">
         <v>-1</v>
@@ -32659,7 +32659,7 @@
         <v>-1</v>
       </c>
       <c r="C24">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D24">
         <v>-1</v>
@@ -32713,7 +32713,7 @@
         <v>-1</v>
       </c>
       <c r="U24">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="V24">
         <v>-1</v>
@@ -33737,7 +33737,7 @@
         <v>-1</v>
       </c>
       <c r="C38">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D38">
         <v>6</v>
@@ -33791,7 +33791,7 @@
         <v>-1</v>
       </c>
       <c r="U38">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="V38">
         <v>6</v>
@@ -33814,7 +33814,7 @@
         <v>6</v>
       </c>
       <c r="C39">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D39">
         <v>6</v>
@@ -33868,7 +33868,7 @@
         <v>6</v>
       </c>
       <c r="U39">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="V39">
         <v>6</v>
@@ -34122,7 +34122,7 @@
         <v>-1</v>
       </c>
       <c r="C43">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D43">
         <v>-1</v>
@@ -34176,7 +34176,7 @@
         <v>-1</v>
       </c>
       <c r="U43">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="V43">
         <v>-1</v>
@@ -35111,7 +35111,7 @@
         <v>6</v>
       </c>
       <c r="D14">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="E14">
         <v>7</v>
@@ -35165,7 +35165,7 @@
         <v>6</v>
       </c>
       <c r="V14">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="W14">
         <v>7</v>
@@ -43557,7 +43557,7 @@
         <v>9</v>
       </c>
       <c r="F45">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="G45">
         <v>-1</v>
@@ -43611,7 +43611,7 @@
         <v>9</v>
       </c>
       <c r="X45">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="Y45">
         <v>-1</v>
@@ -47933,7 +47933,7 @@
         <v>-1</v>
       </c>
       <c r="G5">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H5">
         <v>-1</v>
@@ -47987,7 +47987,7 @@
         <v>-1</v>
       </c>
       <c r="Y5">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -48241,7 +48241,7 @@
         <v>-1</v>
       </c>
       <c r="G9">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H9">
         <v>-1</v>
@@ -48295,7 +48295,7 @@
         <v>-1</v>
       </c>
       <c r="Y9">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -48395,7 +48395,7 @@
         <v>-1</v>
       </c>
       <c r="G11">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H11">
         <v>-1</v>
@@ -48449,7 +48449,7 @@
         <v>-1</v>
       </c>
       <c r="Y11">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -48472,7 +48472,7 @@
         <v>8</v>
       </c>
       <c r="G12">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H12">
         <v>-1</v>
@@ -48526,7 +48526,7 @@
         <v>8</v>
       </c>
       <c r="Y12">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -48549,7 +48549,7 @@
         <v>-1</v>
       </c>
       <c r="G13">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H13">
         <v>-1</v>
@@ -48603,7 +48603,7 @@
         <v>-1</v>
       </c>
       <c r="Y13">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -48626,7 +48626,7 @@
         <v>-1</v>
       </c>
       <c r="G14">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="H14">
         <v>-1</v>
@@ -48680,7 +48680,7 @@
         <v>-1</v>
       </c>
       <c r="Y14">
-        <v>-1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -48703,7 +48703,7 @@
         <v>8</v>
       </c>
       <c r="G15">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H15">
         <v>-1</v>
@@ -48757,7 +48757,7 @@
         <v>8</v>
       </c>
       <c r="Y15">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -48780,7 +48780,7 @@
         <v>-1</v>
       </c>
       <c r="G16">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H16">
         <v>-1</v>
@@ -48834,7 +48834,7 @@
         <v>-1</v>
       </c>
       <c r="Y16">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:25">
@@ -48857,7 +48857,7 @@
         <v>-1</v>
       </c>
       <c r="G17">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H17">
         <v>-1</v>
@@ -48911,7 +48911,7 @@
         <v>-1</v>
       </c>
       <c r="Y17">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:25">
@@ -49011,7 +49011,7 @@
         <v>-1</v>
       </c>
       <c r="G19">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H19">
         <v>-1</v>
@@ -49065,7 +49065,7 @@
         <v>-1</v>
       </c>
       <c r="Y19">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:25">
@@ -49242,7 +49242,7 @@
         <v>7</v>
       </c>
       <c r="G22">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H22">
         <v>-1</v>
@@ -49296,7 +49296,7 @@
         <v>7</v>
       </c>
       <c r="Y22">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:25">
@@ -49319,7 +49319,7 @@
         <v>10</v>
       </c>
       <c r="G23">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H23">
         <v>-1</v>
@@ -49373,7 +49373,7 @@
         <v>10</v>
       </c>
       <c r="Y23">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:25">
@@ -49396,7 +49396,7 @@
         <v>-1</v>
       </c>
       <c r="G24">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H24">
         <v>-1</v>
@@ -49450,7 +49450,7 @@
         <v>-1</v>
       </c>
       <c r="Y24">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:25">
@@ -49550,7 +49550,7 @@
         <v>-1</v>
       </c>
       <c r="G26">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H26">
         <v>-1</v>
@@ -49604,7 +49604,7 @@
         <v>-1</v>
       </c>
       <c r="Y26">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:25">
@@ -49781,7 +49781,7 @@
         <v>9</v>
       </c>
       <c r="G29">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H29">
         <v>-1</v>
@@ -49835,7 +49835,7 @@
         <v>9</v>
       </c>
       <c r="Y29">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:25">
@@ -49858,7 +49858,7 @@
         <v>-1</v>
       </c>
       <c r="G30">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H30">
         <v>-1</v>
@@ -49912,7 +49912,7 @@
         <v>-1</v>
       </c>
       <c r="Y30">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:25">
@@ -49935,7 +49935,7 @@
         <v>-1</v>
       </c>
       <c r="G31">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H31">
         <v>-1</v>
@@ -49989,7 +49989,7 @@
         <v>-1</v>
       </c>
       <c r="Y31">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:25">
@@ -50089,7 +50089,7 @@
         <v>9</v>
       </c>
       <c r="G33">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H33">
         <v>-1</v>
@@ -50143,7 +50143,7 @@
         <v>9</v>
       </c>
       <c r="Y33">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:25">
@@ -50243,7 +50243,7 @@
         <v>9</v>
       </c>
       <c r="G35">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H35">
         <v>-1</v>
@@ -50297,7 +50297,7 @@
         <v>9</v>
       </c>
       <c r="Y35">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:25">
@@ -50320,7 +50320,7 @@
         <v>10</v>
       </c>
       <c r="G36">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H36">
         <v>-1</v>
@@ -50374,7 +50374,7 @@
         <v>10</v>
       </c>
       <c r="Y36">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -57652,7 +57652,7 @@
         <v>7</v>
       </c>
       <c r="G5">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H5">
         <v>-1</v>
@@ -57706,7 +57706,7 @@
         <v>7</v>
       </c>
       <c r="Y5">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -57806,7 +57806,7 @@
         <v>7</v>
       </c>
       <c r="G7">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H7">
         <v>-1</v>
@@ -57860,7 +57860,7 @@
         <v>7</v>
       </c>
       <c r="Y7">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -58114,7 +58114,7 @@
         <v>10</v>
       </c>
       <c r="G11">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="H11">
         <v>-1</v>
@@ -58168,7 +58168,7 @@
         <v>10</v>
       </c>
       <c r="Y11">
-        <v>-1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -58268,7 +58268,7 @@
         <v>8</v>
       </c>
       <c r="G13">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H13">
         <v>-1</v>
@@ -58322,7 +58322,7 @@
         <v>8</v>
       </c>
       <c r="Y13">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -58345,7 +58345,7 @@
         <v>7</v>
       </c>
       <c r="G14">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H14">
         <v>-1</v>
@@ -58399,7 +58399,7 @@
         <v>7</v>
       </c>
       <c r="Y14">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -58576,7 +58576,7 @@
         <v>-1</v>
       </c>
       <c r="G17">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H17">
         <v>-1</v>
@@ -58630,7 +58630,7 @@
         <v>-1</v>
       </c>
       <c r="Y17">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:25">
@@ -58807,7 +58807,7 @@
         <v>-1</v>
       </c>
       <c r="G20">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H20">
         <v>-1</v>
@@ -58861,7 +58861,7 @@
         <v>-1</v>
       </c>
       <c r="Y20">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:25">
@@ -59067,7 +59067,7 @@
         <v>-1</v>
       </c>
       <c r="G24">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H24">
         <v>-1</v>
@@ -59121,7 +59121,7 @@
         <v>-1</v>
       </c>
       <c r="Y24">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:25">
@@ -59144,7 +59144,7 @@
         <v>-1</v>
       </c>
       <c r="G25">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H25">
         <v>-1</v>
@@ -59198,7 +59198,7 @@
         <v>-1</v>
       </c>
       <c r="Y25">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -70118,7 +70118,7 @@
         <v>6</v>
       </c>
       <c r="D4">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="E4">
         <v>8</v>
@@ -70127,7 +70127,7 @@
         <v>7</v>
       </c>
       <c r="G4">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H4">
         <v>-1</v>
@@ -70172,7 +70172,7 @@
         <v>6</v>
       </c>
       <c r="V4">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="W4">
         <v>8</v>
@@ -70181,7 +70181,7 @@
         <v>7</v>
       </c>
       <c r="Y4">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -70281,7 +70281,7 @@
         <v>-1</v>
       </c>
       <c r="G6">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H6">
         <v>-1</v>
@@ -70335,7 +70335,7 @@
         <v>-1</v>
       </c>
       <c r="Y6">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -70503,7 +70503,7 @@
         <v>5</v>
       </c>
       <c r="D9">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="E9">
         <v>-1</v>
@@ -70512,7 +70512,7 @@
         <v>5</v>
       </c>
       <c r="G9">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H9">
         <v>-1</v>
@@ -70557,7 +70557,7 @@
         <v>5</v>
       </c>
       <c r="V9">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="W9">
         <v>-1</v>
@@ -70566,7 +70566,7 @@
         <v>5</v>
       </c>
       <c r="Y9">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -70666,7 +70666,7 @@
         <v>5</v>
       </c>
       <c r="G11">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H11">
         <v>-1</v>
@@ -70720,7 +70720,7 @@
         <v>5</v>
       </c>
       <c r="Y11">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -70734,7 +70734,7 @@
         <v>-1</v>
       </c>
       <c r="D12">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="E12">
         <v>-1</v>
@@ -70743,7 +70743,7 @@
         <v>5</v>
       </c>
       <c r="G12">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H12">
         <v>-1</v>
@@ -70788,7 +70788,7 @@
         <v>-1</v>
       </c>
       <c r="V12">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="W12">
         <v>-1</v>
@@ -70797,7 +70797,7 @@
         <v>5</v>
       </c>
       <c r="Y12">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -71889,7 +71889,7 @@
         <v>6</v>
       </c>
       <c r="D27">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="E27">
         <v>-1</v>
@@ -71898,7 +71898,7 @@
         <v>5</v>
       </c>
       <c r="G27">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H27">
         <v>-1</v>
@@ -71943,7 +71943,7 @@
         <v>6</v>
       </c>
       <c r="V27">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="W27">
         <v>-1</v>
@@ -71952,7 +71952,7 @@
         <v>5</v>
       </c>
       <c r="Y27">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:25">
@@ -71975,7 +71975,7 @@
         <v>-1</v>
       </c>
       <c r="G28">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H28">
         <v>-1</v>
@@ -72029,7 +72029,7 @@
         <v>-1</v>
       </c>
       <c r="Y28">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:25">
@@ -72043,7 +72043,7 @@
         <v>-1</v>
       </c>
       <c r="D29">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="E29">
         <v>-1</v>
@@ -72052,7 +72052,7 @@
         <v>-1</v>
       </c>
       <c r="G29">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H29">
         <v>-1</v>
@@ -72097,7 +72097,7 @@
         <v>-1</v>
       </c>
       <c r="V29">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="W29">
         <v>-1</v>
@@ -72106,7 +72106,7 @@
         <v>-1</v>
       </c>
       <c r="Y29">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:25">
@@ -72197,7 +72197,7 @@
         <v>5</v>
       </c>
       <c r="G31">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="H31">
         <v>-1</v>
@@ -72224,7 +72224,7 @@
         <v>5</v>
       </c>
       <c r="Y31">
-        <v>-1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:25">
@@ -72247,7 +72247,7 @@
         <v>5</v>
       </c>
       <c r="G32">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H32">
         <v>-1</v>
@@ -72301,7 +72301,7 @@
         <v>5</v>
       </c>
       <c r="Y32">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:25">
@@ -72392,7 +72392,7 @@
         <v>-1</v>
       </c>
       <c r="D34">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="E34">
         <v>-1</v>
@@ -72401,7 +72401,7 @@
         <v>5</v>
       </c>
       <c r="G34">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H34">
         <v>-1</v>
@@ -72446,7 +72446,7 @@
         <v>-1</v>
       </c>
       <c r="V34">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="W34">
         <v>-1</v>
@@ -72455,7 +72455,7 @@
         <v>5</v>
       </c>
       <c r="Y34">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:25">
@@ -72694,13 +72694,13 @@
         <v>1086</v>
       </c>
       <c r="D38">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="F38">
         <v>5</v>
       </c>
       <c r="G38">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="J38">
         <v>-1</v>
@@ -72721,13 +72721,13 @@
         <v>-1</v>
       </c>
       <c r="V38">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="X38">
         <v>5</v>
       </c>
       <c r="Y38">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:25">
@@ -72827,7 +72827,7 @@
         <v>-1</v>
       </c>
       <c r="G40">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H40">
         <v>-1</v>
@@ -72881,7 +72881,7 @@
         <v>-1</v>
       </c>
       <c r="Y40">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>